<commit_message>
Delete Student - Done!
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF68AE0-B8BC-4D4B-BFFA-30A8938FA343}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B25DE518-4F08-4A08-96AB-40F20A7CFAC1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="3" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="9" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="234">
   <si>
     <t>SID</t>
   </si>
@@ -722,6 +722,24 @@
   <si>
     <t>TBL_Classes_FindStudent</t>
   </si>
+  <si>
+    <t>T_sid_DeleteStudent</t>
+  </si>
+  <si>
+    <t>B_Delete_DeleteStudent</t>
+  </si>
+  <si>
+    <t>B_Cancel_DeleteStudent</t>
+  </si>
+  <si>
+    <t>L_Error_DeleteStudent</t>
+  </si>
+  <si>
+    <t>trigger</t>
+  </si>
+  <si>
+    <t>L_Message_DeleteStudent</t>
+  </si>
 </sst>
 </file>
 
@@ -814,7 +832,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -884,43 +902,6 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -943,11 +924,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1043,12 +1037,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1626,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA49FE7-C6D8-47F3-B9B5-3C10CD53B227}">
-  <dimension ref="A1:XFD20"/>
+  <dimension ref="A1:XFD21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1640,16 +1628,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
     </row>
     <row r="3" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
@@ -1813,7 +1803,7 @@
     </row>
     <row r="13" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="29"/>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="30" t="s">
         <v>206</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -1829,7 +1819,7 @@
     </row>
     <row r="14" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="29"/>
-      <c r="B14" s="34"/>
+      <c r="B14" s="31"/>
       <c r="C14" s="20" t="s">
         <v>213</v>
       </c>
@@ -1845,7 +1835,7 @@
     </row>
     <row r="15" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
-      <c r="B15" s="34"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="20" t="s">
         <v>220</v>
       </c>
@@ -1859,7 +1849,7 @@
     </row>
     <row r="16" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29"/>
-      <c r="B16" s="34"/>
+      <c r="B16" s="31"/>
       <c r="C16" s="26" t="s">
         <v>216</v>
       </c>
@@ -18261,7 +18251,7 @@
     </row>
     <row r="17" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
-      <c r="B17" s="34"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="26" t="s">
         <v>217</v>
       </c>
@@ -34665,10 +34655,12 @@
     </row>
     <row r="19" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29"/>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="C19" s="20"/>
+      <c r="C19" s="20" t="s">
+        <v>228</v>
+      </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
@@ -34679,9 +34671,13 @@
     </row>
     <row r="20" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="29"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="20" t="s">
+        <v>231</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>233</v>
+      </c>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
       <c r="G20" s="20"/>
@@ -34689,13 +34685,30 @@
       <c r="I20" s="20"/>
       <c r="J20" s="20"/>
     </row>
+    <row r="21" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A5:A20"/>
+    <mergeCell ref="A5:A21"/>
     <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A1:H1"/>
     <mergeCell ref="B13:B17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -35012,7 +35025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7971D23-0DFC-4F8A-B695-C4DE9A893734}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -35861,9 +35874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718F9279-C340-4770-88F1-01842C5185FC}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -35876,7 +35889,7 @@
     <col min="14" max="16384" width="15.77734375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="12" t="s">
         <v>133</v>
       </c>
@@ -35890,7 +35903,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14">
         <v>1</v>
       </c>
@@ -35904,7 +35917,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34.35" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="34.35" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14">
         <v>2</v>
       </c>
@@ -35918,7 +35931,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="66" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14">
         <v>3</v>
       </c>
@@ -35932,7 +35945,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="63.15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="63.15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14">
         <v>4</v>
       </c>
@@ -35946,7 +35959,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="14">
         <v>5</v>
       </c>
@@ -35960,7 +35973,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
         <v>6</v>
       </c>
@@ -35974,7 +35987,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="91.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14">
         <v>7</v>
       </c>
@@ -35988,7 +36001,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14">
         <v>8</v>
       </c>
@@ -36001,8 +36014,11 @@
       <c r="D9" s="15" t="s">
         <v>151</v>
       </c>
+      <c r="E9" s="9" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>

</xml_diff>

<commit_message>
Find Course - GUI part 1 done
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F054B51-33FC-4AE5-8D4B-6B91E3596C87}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21723BD6-8CDD-46F7-B55F-9A1E73B0A86C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="10" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="2" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="258">
   <si>
     <t>SID</t>
   </si>
@@ -794,6 +794,24 @@
   </si>
   <si>
     <t>TBL_ShowAllPre</t>
+  </si>
+  <si>
+    <t>T_Course_FindCourse</t>
+  </si>
+  <si>
+    <t>T_Dept_FindCourse</t>
+  </si>
+  <si>
+    <t>L_Error_FindCourse</t>
+  </si>
+  <si>
+    <t>B_Find_FindCourse</t>
+  </si>
+  <si>
+    <t>B_Cancel_FindCourse</t>
+  </si>
+  <si>
+    <t>P_CourseDetails_FindCourse</t>
   </si>
 </sst>
 </file>
@@ -34839,8 +34857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98460CC7-C1E9-450B-B05B-F40B8C1CECD1}">
   <dimension ref="A1:XFD21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34999,8 +35017,12 @@
       <c r="B13" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>252</v>
+      </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
       <c r="G13" s="20"/>
@@ -35011,7 +35033,9 @@
     <row r="14" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="35"/>
       <c r="B14" s="38"/>
-      <c r="C14" s="20"/>
+      <c r="C14" s="20" t="s">
+        <v>254</v>
+      </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -35023,8 +35047,12 @@
     <row r="15" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="35"/>
       <c r="B15" s="38"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="C15" s="20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>256</v>
+      </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
       <c r="G15" s="20"/>
@@ -35035,7 +35063,9 @@
     <row r="16" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="30"/>
+      <c r="C16" s="30" t="s">
+        <v>257</v>
+      </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
@@ -68006,8 +68036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985EAC5D-1F57-41D9-8085-63ADF5A18429}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69019,7 +69049,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69310,13 +69340,13 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.77734375" style="1"/>
-    <col min="2" max="2" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.77734375" style="1"/>
     <col min="5" max="5" width="17.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -69498,8 +69528,20 @@
       <c r="B10" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="7" t="s">
         <v>178</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="29" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -69507,10 +69549,34 @@
       <c r="B11" s="32" t="s">
         <v>163</v>
       </c>
+      <c r="C11" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="E11" s="29" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="12" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
+      <c r="C12" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">

</xml_diff>

<commit_message>
Find Course - Done!
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21723BD6-8CDD-46F7-B55F-9A1E73B0A86C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0990FAC0-1258-4799-B8F5-1ACA143DB230}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="2" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="10" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="260">
   <si>
     <t>SID</t>
   </si>
@@ -811,7 +811,13 @@
     <t>B_Cancel_FindCourse</t>
   </si>
   <si>
-    <t>P_CourseDetails_FindCourse</t>
+    <t>L_Message_FindCourse</t>
+  </si>
+  <si>
+    <t>TBL_ShowPre_FindCourse</t>
+  </si>
+  <si>
+    <t>P_ShowPre_FindCourse</t>
   </si>
 </sst>
 </file>
@@ -913,7 +919,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1036,11 +1042,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1129,10 +1166,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1157,6 +1194,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1737,7 +1786,7 @@
   <dimension ref="A1:XFD23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -34855,20 +34904,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98460CC7-C1E9-450B-B05B-F40B8C1CECD1}">
-  <dimension ref="A1:XFD21"/>
+  <dimension ref="A1:XEY17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="25.77734375" style="19"/>
-    <col min="3" max="10" width="30.77734375" style="19" customWidth="1"/>
-    <col min="11" max="16384" width="25.77734375" style="19"/>
+    <col min="3" max="5" width="30.77734375" style="19" customWidth="1"/>
+    <col min="6" max="16384" width="25.77734375" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="33" t="s">
         <v>235</v>
       </c>
@@ -34876,14 +34925,16 @@
       <c r="C1" s="33"/>
       <c r="D1" s="33"/>
       <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
     </row>
-    <row r="3" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+    <row r="2" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="43"/>
+    </row>
+    <row r="3" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
         <v>236</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -34898,34 +34949,34 @@
       <c r="E3" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
     </row>
-    <row r="5" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34" t="s">
+    <row r="4" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="27"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="43"/>
+    </row>
+    <row r="5" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>242</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
     </row>
-    <row r="6" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="35"/>
+    <row r="6" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="41"/>
       <c r="B6" s="23"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="43"/>
     </row>
-    <row r="7" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="35"/>
+    <row r="7" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="41"/>
       <c r="B7" s="33" t="s">
         <v>243</v>
       </c>
@@ -34934,42 +34985,27 @@
       </c>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
     </row>
-    <row r="8" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="35"/>
+    <row r="8" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="41"/>
       <c r="B8" s="33"/>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="31" t="s">
         <v>245</v>
       </c>
       <c r="D8" s="20" t="s">
         <v>246</v>
       </c>
       <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
     </row>
-    <row r="9" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="35"/>
+    <row r="9" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="41"/>
       <c r="B9" s="23"/>
       <c r="C9" s="24"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="25"/>
+      <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="35"/>
+    <row r="10" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="41"/>
       <c r="B10" s="33" t="s">
         <v>248</v>
       </c>
@@ -34978,42 +35014,27 @@
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
     </row>
-    <row r="11" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="35"/>
+    <row r="11" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="41"/>
       <c r="B11" s="33"/>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="31" t="s">
         <v>250</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>251</v>
       </c>
       <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
     </row>
-    <row r="12" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="35"/>
+    <row r="12" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="41"/>
       <c r="B12" s="23"/>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="25"/>
+      <c r="E12" s="25"/>
     </row>
-    <row r="13" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="35"/>
+    <row r="13" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="41"/>
       <c r="B13" s="37" t="s">
         <v>247</v>
       </c>
@@ -35024,28 +35045,18 @@
         <v>252</v>
       </c>
       <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
     </row>
-    <row r="14" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="35"/>
+    <row r="14" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="41"/>
       <c r="B14" s="38"/>
       <c r="C14" s="20" t="s">
         <v>254</v>
       </c>
       <c r="D14" s="20"/>
       <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
     </row>
-    <row r="15" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="35"/>
+    <row r="15" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="41"/>
       <c r="B15" s="38"/>
       <c r="C15" s="20" t="s">
         <v>255</v>
@@ -35054,25 +35065,20 @@
         <v>256</v>
       </c>
       <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
     </row>
-    <row r="16" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="35"/>
+    <row r="16" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="41"/>
       <c r="B16" s="38"/>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="20" t="s">
         <v>257</v>
       </c>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
+      <c r="F16" s="27"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
       <c r="K16" s="27"/>
       <c r="L16" s="27"/>
       <c r="M16" s="27"/>
@@ -51442,23 +51448,22 @@
       <c r="XEW16" s="27"/>
       <c r="XEX16" s="27"/>
       <c r="XEY16" s="27"/>
-      <c r="XEZ16" s="27"/>
-      <c r="XFA16" s="27"/>
-      <c r="XFB16" s="27"/>
-      <c r="XFC16" s="27"/>
-      <c r="XFD16" s="27"/>
     </row>
-    <row r="17" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="35"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="20"/>
+    <row r="17" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="42"/>
+      <c r="B17" s="39"/>
+      <c r="C17" s="31" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>258</v>
+      </c>
       <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
       <c r="K17" s="27"/>
       <c r="L17" s="27"/>
       <c r="M17" s="27"/>
@@ -67828,68 +67833,14 @@
       <c r="XEW17" s="27"/>
       <c r="XEX17" s="27"/>
       <c r="XEY17" s="27"/>
-      <c r="XEZ17" s="27"/>
-      <c r="XFA17" s="27"/>
-      <c r="XFB17" s="27"/>
-      <c r="XFC17" s="27"/>
-      <c r="XFD17" s="27"/>
-    </row>
-    <row r="18" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="35"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="25"/>
-    </row>
-    <row r="19" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
-      <c r="B19" s="37"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-    </row>
-    <row r="20" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
-      <c r="B20" s="38"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-    </row>
-    <row r="21" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="36"/>
-      <c r="B21" s="39"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A5:A21"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A5:A17"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="B13:B17"/>
-    <mergeCell ref="B19:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -67901,7 +67852,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -67920,6 +67871,9 @@
       </c>
       <c r="C1" s="3" t="s">
         <v>43</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>93</v>
@@ -67940,6 +67894,9 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>47</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>95</v>
@@ -67963,6 +67920,9 @@
       </c>
       <c r="C3" s="3" t="s">
         <v>48</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>88</v>
@@ -68036,8 +67996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{985EAC5D-1F57-41D9-8085-63ADF5A18429}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:K6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69049,7 +69009,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69340,7 +69300,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B16"/>
+      <selection activeCell="K9" sqref="K9:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69383,7 +69343,7 @@
       <c r="I1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="30" t="s">
         <v>212</v>
       </c>
       <c r="K1" s="7"/>
@@ -69500,7 +69460,7 @@
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
-      <c r="L7" s="31"/>
+      <c r="L7" s="30"/>
       <c r="M7" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Show Enrollments - Done!
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C399B1-950C-47CC-87AC-D2FE00D7A6D9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45520FA8-E38D-4D4A-A1BC-B63D4588336E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" activeTab="11" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" firstSheet="1" activeTab="12" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Manage Students" sheetId="12" r:id="rId10"/>
     <sheet name="View Courses" sheetId="13" r:id="rId11"/>
     <sheet name="View Classes" sheetId="14" r:id="rId12"/>
+    <sheet name="Manage Enrollments" sheetId="15" r:id="rId13"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="304">
   <si>
     <t>SID</t>
   </si>
@@ -910,6 +911,48 @@
   <si>
     <t>TBL_Students_FindClass</t>
   </si>
+  <si>
+    <t>P_ManageEnrollments</t>
+  </si>
+  <si>
+    <t>P_Button_Enrollments</t>
+  </si>
+  <si>
+    <t>B_ShowAllEnrollments</t>
+  </si>
+  <si>
+    <t>B_EnrollStudent</t>
+  </si>
+  <si>
+    <t>B_DropEnrollment</t>
+  </si>
+  <si>
+    <t>B_ExitEnrollments</t>
+  </si>
+  <si>
+    <t>LP_Enrollments</t>
+  </si>
+  <si>
+    <t>P_Default_Enrollments</t>
+  </si>
+  <si>
+    <t>P_ShowAllEnrollments</t>
+  </si>
+  <si>
+    <t>L_Message_ShowAllEnrollments</t>
+  </si>
+  <si>
+    <t>P_Table_ShowAllEnrollments</t>
+  </si>
+  <si>
+    <t>TBL_ShowAllEnrollments</t>
+  </si>
+  <si>
+    <t>P_EnrollStudent</t>
+  </si>
+  <si>
+    <t>P_DropEnrollment</t>
+  </si>
 </sst>
 </file>
 
@@ -1181,7 +1224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1291,6 +1334,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1322,12 +1374,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1919,18 +1965,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
     </row>
     <row r="3" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
@@ -1957,7 +2003,7 @@
       <c r="J3" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="42" t="s">
         <v>186</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -1973,12 +2019,12 @@
       <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
+      <c r="A6" s="43"/>
       <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="43"/>
+      <c r="B7" s="41" t="s">
         <v>184</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -1993,8 +2039,8 @@
       <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="40"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="20" t="s">
         <v>210</v>
       </c>
@@ -2009,7 +2055,7 @@
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40"/>
+      <c r="A9" s="43"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -2021,8 +2067,8 @@
       <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
-      <c r="B10" s="38" t="s">
+      <c r="A10" s="43"/>
+      <c r="B10" s="41" t="s">
         <v>185</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -2043,8 +2089,8 @@
       <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="20" t="s">
         <v>190</v>
       </c>
@@ -2067,8 +2113,8 @@
       <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="38"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="19" t="s">
         <v>204</v>
       </c>
@@ -2083,8 +2129,8 @@
       <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="40"/>
-      <c r="B13" s="38"/>
+      <c r="A13" s="43"/>
+      <c r="B13" s="41"/>
       <c r="C13" s="19" t="s">
         <v>203</v>
       </c>
@@ -2099,7 +2145,7 @@
       <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40"/>
+      <c r="A14" s="43"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -2111,8 +2157,8 @@
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="42" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="45" t="s">
         <v>206</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -2127,8 +2173,8 @@
       <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="43"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="19" t="s">
         <v>213</v>
       </c>
@@ -2143,8 +2189,8 @@
       <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="40"/>
-      <c r="B17" s="43"/>
+      <c r="A17" s="43"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="19" t="s">
         <v>220</v>
       </c>
@@ -2157,8 +2203,8 @@
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40"/>
-      <c r="B18" s="43"/>
+      <c r="A18" s="43"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="25" t="s">
         <v>216</v>
       </c>
@@ -18559,8 +18605,8 @@
       <c r="XFD18" s="26"/>
     </row>
     <row r="19" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="43"/>
+      <c r="A19" s="43"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="25" t="s">
         <v>217</v>
       </c>
@@ -34951,7 +34997,7 @@
       <c r="XFD19" s="26"/>
     </row>
     <row r="20" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
+      <c r="A20" s="43"/>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
@@ -34963,8 +35009,8 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
-      <c r="B21" s="42" t="s">
+      <c r="A21" s="43"/>
+      <c r="B21" s="45" t="s">
         <v>207</v>
       </c>
       <c r="C21" s="19" t="s">
@@ -34979,8 +35025,8 @@
       <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
-      <c r="B22" s="43"/>
+      <c r="A22" s="43"/>
+      <c r="B22" s="46"/>
       <c r="C22" s="19" t="s">
         <v>231</v>
       </c>
@@ -34995,8 +35041,8 @@
       <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="41"/>
-      <c r="B23" s="44"/>
+      <c r="A23" s="44"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="19" t="s">
         <v>229</v>
       </c>
@@ -35040,13 +35086,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -35080,7 +35126,7 @@
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="48" t="s">
         <v>241</v>
       </c>
       <c r="B5" s="30" t="s">
@@ -35091,15 +35137,15 @@
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="41" t="s">
         <v>243</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -35109,8 +35155,8 @@
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="30" t="s">
         <v>245</v>
       </c>
@@ -35120,15 +35166,15 @@
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="38" t="s">
+      <c r="A10" s="49"/>
+      <c r="B10" s="41" t="s">
         <v>248</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -35138,8 +35184,8 @@
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
-      <c r="B11" s="38"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="30" t="s">
         <v>250</v>
       </c>
@@ -35149,15 +35195,15 @@
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
-      <c r="B13" s="42" t="s">
+      <c r="A13" s="49"/>
+      <c r="B13" s="45" t="s">
         <v>247</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -35169,8 +35215,8 @@
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="46"/>
       <c r="C14" s="19" t="s">
         <v>254</v>
       </c>
@@ -35178,8 +35224,8 @@
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="46"/>
-      <c r="B15" s="43"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="46"/>
       <c r="C15" s="19" t="s">
         <v>255</v>
       </c>
@@ -35189,8 +35235,8 @@
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46"/>
-      <c r="B16" s="43"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="19" t="s">
         <v>257</v>
       </c>
@@ -51572,8 +51618,8 @@
       <c r="XEY16" s="26"/>
     </row>
     <row r="17" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="47"/>
-      <c r="B17" s="44"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="30" t="s">
         <v>259</v>
       </c>
@@ -67973,7 +68019,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6DB7A06-221F-4E56-A87F-FC8A2DB02451}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:B14"/>
     </sheetView>
   </sheetViews>
@@ -67985,20 +68031,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="41" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
     </row>
     <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -68051,7 +68097,7 @@
       <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="45" t="s">
+      <c r="A5" s="48" t="s">
         <v>268</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -68069,7 +68115,7 @@
       <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -68083,8 +68129,8 @@
       <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
-      <c r="B7" s="38" t="s">
+      <c r="A7" s="49"/>
+      <c r="B7" s="41" t="s">
         <v>261</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -68101,8 +68147,8 @@
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
-      <c r="B8" s="38"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="41"/>
       <c r="C8" s="31" t="s">
         <v>270</v>
       </c>
@@ -68119,22 +68165,22 @@
       <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="49"/>
-      <c r="G9" s="49"/>
-      <c r="H9" s="49"/>
-      <c r="I9" s="49"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
       <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="49"/>
+      <c r="B10" s="45" t="s">
         <v>262</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -68151,8 +68197,8 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
-      <c r="B11" s="43"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="46"/>
       <c r="C11" s="19" t="s">
         <v>274</v>
       </c>
@@ -68169,8 +68215,8 @@
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
-      <c r="B12" s="43"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="46"/>
       <c r="C12" s="19" t="s">
         <v>276</v>
       </c>
@@ -68185,8 +68231,8 @@
       <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
-      <c r="B13" s="43"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="46"/>
       <c r="C13" s="33" t="s">
         <v>277</v>
       </c>
@@ -68219,8 +68265,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="47"/>
-      <c r="B14" s="44"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="33" t="s">
         <v>278</v>
       </c>
@@ -68244,6 +68290,354 @@
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4947D9BD-9EC3-4FDB-A350-33C06B093680}">
+  <dimension ref="A1:L20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="25.77734375" style="18"/>
+    <col min="3" max="12" width="30.77734375" style="18" customWidth="1"/>
+    <col min="13" max="16384" width="25.77734375" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
+        <v>290</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+    </row>
+    <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="32"/>
+    </row>
+    <row r="3" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="37" t="s">
+        <v>291</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="32"/>
+    </row>
+    <row r="5" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="48" t="s">
+        <v>296</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="19"/>
+      <c r="L5" s="19"/>
+    </row>
+    <row r="6" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="49"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="32"/>
+    </row>
+    <row r="7" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>299</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+    </row>
+    <row r="8" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="49"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="37" t="s">
+        <v>300</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>301</v>
+      </c>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="49"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="24"/>
+    </row>
+    <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="49"/>
+      <c r="B10" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+    </row>
+    <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="49"/>
+      <c r="B11" s="46"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+    </row>
+    <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="49"/>
+      <c r="B12" s="46"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="49"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
+      <c r="I13" s="19"/>
+      <c r="J13" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="K13" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="L13" s="19" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
+      <c r="I14" s="19"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="49"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="24"/>
+    </row>
+    <row r="16" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="49"/>
+      <c r="B16" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="49"/>
+      <c r="B17" s="46"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49"/>
+      <c r="B18" s="46"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+    </row>
+    <row r="19" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="K19" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="L19" s="19" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="50"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="A5:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -68886,7 +69280,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:A18"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69700,7 +70094,7 @@
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16:G16"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69716,7 +70110,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>157</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -69751,8 +70145,8 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="37"/>
-      <c r="B2" s="37" t="s">
+      <c r="A2" s="40"/>
+      <c r="B2" s="40" t="s">
         <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -69780,8 +70174,8 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="40"/>
+      <c r="B3" s="40"/>
       <c r="C3" s="34" t="s">
         <v>178</v>
       </c>
@@ -69797,8 +70191,8 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="37"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="40" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -69816,8 +70210,8 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="37"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="34" t="s">
         <v>178</v>
       </c>
@@ -69847,8 +70241,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="37"/>
-      <c r="B6" s="37" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="40" t="s">
         <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -69866,8 +70260,8 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="40"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="34" t="s">
         <v>178</v>
       </c>
@@ -69885,7 +70279,7 @@
       <c r="M7" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="40" t="s">
         <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -69906,7 +70300,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="37"/>
+      <c r="A10" s="40"/>
       <c r="B10" s="2" t="s">
         <v>160</v>
       </c>
@@ -69927,8 +70321,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="28" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="37"/>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="40" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -69944,8 +70338,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="37"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="34" t="s">
         <v>178</v>
       </c>
@@ -69963,7 +70357,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="40" t="s">
         <v>164</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -69998,8 +70392,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="37"/>
-      <c r="B15" s="37" t="s">
+      <c r="A15" s="40"/>
+      <c r="B15" s="40" t="s">
         <v>165</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -70017,8 +70411,8 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="37"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="34" t="s">
         <v>178</v>
       </c>
@@ -70044,7 +70438,7 @@
       <c r="K16" s="2"/>
     </row>
     <row r="18" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="48" t="s">
+      <c r="A18" s="39" t="s">
         <v>168</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -70052,13 +70446,13 @@
       </c>
     </row>
     <row r="19" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="1" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
+      <c r="A20" s="39"/>
       <c r="B20" s="1" t="s">
         <v>170</v>
       </c>

</xml_diff>

<commit_message>
Added procedure for Enroll Student. Updated indexing for .sql file, for better scope understanding.
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45520FA8-E38D-4D4A-A1BC-B63D4588336E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E747B4D-4E7F-479B-9F74-BFF8814C2D7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" firstSheet="1" activeTab="12" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" firstSheet="1" activeTab="6" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="310">
   <si>
     <t>SID</t>
   </si>
@@ -952,6 +952,24 @@
   </si>
   <si>
     <t>P_DropEnrollment</t>
+  </si>
+  <si>
+    <t>T_sid_EnrollStudent</t>
+  </si>
+  <si>
+    <t>T_cid_EnrollStudent</t>
+  </si>
+  <si>
+    <t>B_Enroll_EnrollStudent</t>
+  </si>
+  <si>
+    <t>B_Cancel_EnrollStudent</t>
+  </si>
+  <si>
+    <t>L_Error_EnrollStudent</t>
+  </si>
+  <si>
+    <t>L_Message_EnrollStudent</t>
   </si>
 </sst>
 </file>
@@ -68020,7 +68038,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -68298,10 +68316,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4947D9BD-9EC3-4FDB-A350-33C06B093680}">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -68466,8 +68484,12 @@
       <c r="B10" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
+      <c r="C10" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>305</v>
+      </c>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
       <c r="G10" s="19"/>
@@ -68480,8 +68502,12 @@
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="49"/>
       <c r="B11" s="46"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="19"/>
+      <c r="C11" s="19" t="s">
+        <v>306</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>307</v>
+      </c>
       <c r="E11" s="19"/>
       <c r="F11" s="19"/>
       <c r="G11" s="19"/>
@@ -68494,7 +68520,9 @@
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="49"/>
       <c r="B12" s="46"/>
-      <c r="C12" s="19"/>
+      <c r="C12" s="19" t="s">
+        <v>308</v>
+      </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
       <c r="F12" s="19"/>
@@ -68508,7 +68536,9 @@
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="49"/>
       <c r="B13" s="46"/>
-      <c r="C13" s="37"/>
+      <c r="C13" s="19" t="s">
+        <v>309</v>
+      </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
       <c r="F13" s="19"/>
@@ -68527,37 +68557,37 @@
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49"/>
-      <c r="B14" s="47"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="24"/>
     </row>
     <row r="15" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="49"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="23"/>
-      <c r="K15" s="23"/>
-      <c r="L15" s="24"/>
+      <c r="B15" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="49"/>
-      <c r="B16" s="45" t="s">
-        <v>303</v>
-      </c>
+      <c r="B16" s="46"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -68586,20 +68616,26 @@
     <row r="18" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49"/>
       <c r="B18" s="46"/>
-      <c r="C18" s="19"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
       <c r="F18" s="19"/>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
       <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
-      <c r="L18" s="19"/>
+      <c r="J18" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="K18" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="L18" s="19" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="50"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="37"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
@@ -68607,37 +68643,17 @@
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
-      <c r="J19" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="K19" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="50"/>
-      <c r="B20" s="47"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="A5:A20"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="A5:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -68956,7 +68972,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69280,7 +69296,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69801,9 +69817,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718F9279-C340-4770-88F1-01842C5185FC}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Enroll Students - Done!
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E747B4D-4E7F-479B-9F74-BFF8814C2D7C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC417E1-77DB-474E-890F-FCA7A0DD7C0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" firstSheet="1" activeTab="6" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" firstSheet="1" activeTab="8" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="310">
   <si>
     <t>SID</t>
   </si>
@@ -1242,7 +1242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1361,6 +1361,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1392,6 +1395,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1983,18 +1989,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="3" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
@@ -2021,7 +2027,7 @@
       <c r="J3" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="43" t="s">
         <v>186</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -2037,12 +2043,12 @@
       <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="43"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="43"/>
-      <c r="B7" s="41" t="s">
+      <c r="A7" s="44"/>
+      <c r="B7" s="42" t="s">
         <v>184</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -2057,8 +2063,8 @@
       <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="43"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="20" t="s">
         <v>210</v>
       </c>
@@ -2073,7 +2079,7 @@
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="43"/>
+      <c r="A9" s="44"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -2085,8 +2091,8 @@
       <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43"/>
-      <c r="B10" s="41" t="s">
+      <c r="A10" s="44"/>
+      <c r="B10" s="42" t="s">
         <v>185</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -2107,8 +2113,8 @@
       <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="43"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="44"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="20" t="s">
         <v>190</v>
       </c>
@@ -2131,8 +2137,8 @@
       <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="43"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="44"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="19" t="s">
         <v>204</v>
       </c>
@@ -2147,8 +2153,8 @@
       <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="43"/>
-      <c r="B13" s="41"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="42"/>
       <c r="C13" s="19" t="s">
         <v>203</v>
       </c>
@@ -2163,7 +2169,7 @@
       <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
+      <c r="A14" s="44"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -2175,8 +2181,8 @@
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="43"/>
-      <c r="B15" s="45" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="46" t="s">
         <v>206</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -2191,8 +2197,8 @@
       <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="43"/>
-      <c r="B16" s="46"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="19" t="s">
         <v>213</v>
       </c>
@@ -2207,8 +2213,8 @@
       <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="43"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="19" t="s">
         <v>220</v>
       </c>
@@ -2221,8 +2227,8 @@
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="25" t="s">
         <v>216</v>
       </c>
@@ -18623,8 +18629,8 @@
       <c r="XFD18" s="26"/>
     </row>
     <row r="19" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="44"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="25" t="s">
         <v>217</v>
       </c>
@@ -35015,7 +35021,7 @@
       <c r="XFD19" s="26"/>
     </row>
     <row r="20" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="43"/>
+      <c r="A20" s="44"/>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
@@ -35027,8 +35033,8 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="43"/>
-      <c r="B21" s="45" t="s">
+      <c r="A21" s="44"/>
+      <c r="B21" s="46" t="s">
         <v>207</v>
       </c>
       <c r="C21" s="19" t="s">
@@ -35043,8 +35049,8 @@
       <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="43"/>
-      <c r="B22" s="46"/>
+      <c r="A22" s="44"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="19" t="s">
         <v>231</v>
       </c>
@@ -35059,8 +35065,8 @@
       <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="44"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="45"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="19" t="s">
         <v>229</v>
       </c>
@@ -35104,13 +35110,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
     </row>
     <row r="2" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -35144,7 +35150,7 @@
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="49" t="s">
         <v>241</v>
       </c>
       <c r="B5" s="30" t="s">
@@ -35155,15 +35161,15 @@
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="41" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="42" t="s">
         <v>243</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -35173,8 +35179,8 @@
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="30" t="s">
         <v>245</v>
       </c>
@@ -35184,15 +35190,15 @@
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="41" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="42" t="s">
         <v>248</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -35202,8 +35208,8 @@
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="41"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="42"/>
       <c r="C11" s="30" t="s">
         <v>250</v>
       </c>
@@ -35213,15 +35219,15 @@
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
+      <c r="A12" s="50"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="45" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="46" t="s">
         <v>247</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -35233,8 +35239,8 @@
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="46"/>
+      <c r="A14" s="50"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="19" t="s">
         <v>254</v>
       </c>
@@ -35242,8 +35248,8 @@
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="46"/>
+      <c r="A15" s="50"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="19" t="s">
         <v>255</v>
       </c>
@@ -35253,8 +35259,8 @@
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="46"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="19" t="s">
         <v>257</v>
       </c>
@@ -51636,8 +51642,8 @@
       <c r="XEY16" s="26"/>
     </row>
     <row r="17" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="51"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="30" t="s">
         <v>259</v>
       </c>
@@ -68049,20 +68055,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -68115,7 +68121,7 @@
       <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="49" t="s">
         <v>268</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -68133,7 +68139,7 @@
       <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -68147,8 +68153,8 @@
       <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="41" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="42" t="s">
         <v>261</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -68165,8 +68171,8 @@
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="31" t="s">
         <v>270</v>
       </c>
@@ -68183,7 +68189,7 @@
       <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -68197,8 +68203,8 @@
       <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="46" t="s">
         <v>262</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -68215,8 +68221,8 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="46"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="19" t="s">
         <v>274</v>
       </c>
@@ -68233,8 +68239,8 @@
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="46"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="19" t="s">
         <v>276</v>
       </c>
@@ -68249,8 +68255,8 @@
       <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="46"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="33" t="s">
         <v>277</v>
       </c>
@@ -68283,8 +68289,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="47"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="33" t="s">
         <v>278</v>
       </c>
@@ -68330,20 +68336,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="41"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
     </row>
     <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -68398,7 +68404,7 @@
       <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="49" t="s">
         <v>296</v>
       </c>
       <c r="B5" s="37" t="s">
@@ -68416,7 +68422,7 @@
       <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
+      <c r="A6" s="50"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -68430,8 +68436,8 @@
       <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="41" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="42" t="s">
         <v>298</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -68448,8 +68454,8 @@
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="41"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="42"/>
       <c r="C8" s="37" t="s">
         <v>300</v>
       </c>
@@ -68466,7 +68472,7 @@
       <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
+      <c r="A9" s="50"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -68480,8 +68486,8 @@
       <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="49"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="46" t="s">
         <v>302</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -68500,8 +68506,8 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="46"/>
+      <c r="A11" s="50"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="19" t="s">
         <v>306</v>
       </c>
@@ -68518,8 +68524,8 @@
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="46"/>
+      <c r="A12" s="50"/>
+      <c r="B12" s="47"/>
       <c r="C12" s="19" t="s">
         <v>308</v>
       </c>
@@ -68534,8 +68540,8 @@
       <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="46"/>
+      <c r="A13" s="50"/>
+      <c r="B13" s="47"/>
       <c r="C13" s="19" t="s">
         <v>309</v>
       </c>
@@ -68556,7 +68562,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
+      <c r="A14" s="50"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -68570,8 +68576,8 @@
       <c r="L14" s="24"/>
     </row>
     <row r="15" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="49"/>
-      <c r="B15" s="45" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="46" t="s">
         <v>303</v>
       </c>
       <c r="C15" s="19"/>
@@ -68586,8 +68592,8 @@
       <c r="L15" s="19"/>
     </row>
     <row r="16" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="46"/>
+      <c r="A16" s="50"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -68600,8 +68606,8 @@
       <c r="L16" s="19"/>
     </row>
     <row r="17" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="50"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -68614,8 +68620,8 @@
       <c r="L17" s="19"/>
     </row>
     <row r="18" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="50"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="37"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -68634,8 +68640,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="50"/>
-      <c r="B19" s="47"/>
+      <c r="A19" s="51"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="37"/>
       <c r="D19" s="19"/>
       <c r="E19" s="19"/>
@@ -68810,7 +68816,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -68972,7 +68978,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69296,7 +69302,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H7" sqref="H7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -69388,13 +69394,13 @@
     </row>
     <row r="4" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="1"/>
@@ -69408,10 +69414,10 @@
     </row>
     <row r="5" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>72</v>
@@ -69428,13 +69434,13 @@
     </row>
     <row r="6" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="1"/>
@@ -69448,17 +69454,14 @@
     </row>
     <row r="7" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -69468,10 +69471,10 @@
     </row>
     <row r="8" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>71</v>
@@ -69529,7 +69532,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>72</v>
@@ -69546,13 +69549,13 @@
     </row>
     <row r="12" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="1"/>
@@ -69566,10 +69569,10 @@
     </row>
     <row r="13" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>72</v>
@@ -69586,7 +69589,7 @@
     </row>
     <row r="14" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>69</v>
@@ -69606,10 +69609,10 @@
     </row>
     <row r="15" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>71</v>
@@ -69626,13 +69629,13 @@
     </row>
     <row r="16" spans="1:16" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>69</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="1"/>
@@ -69646,13 +69649,13 @@
     </row>
     <row r="17" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
@@ -69668,7 +69671,7 @@
     </row>
   </sheetData>
   <sortState ref="A2:C18">
-    <sortCondition ref="B2:B18"/>
+    <sortCondition ref="A2:A18"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -69817,7 +69820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718F9279-C340-4770-88F1-01842C5185FC}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -70107,10 +70110,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4014D9C3-5F07-4F82-A3CA-A19916A85FB5}">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -70126,7 +70129,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>157</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -70161,8 +70164,8 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40" t="s">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41" t="s">
         <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -70190,8 +70193,8 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
       <c r="C3" s="34" t="s">
         <v>178</v>
       </c>
@@ -70207,8 +70210,8 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40" t="s">
+      <c r="A4" s="41"/>
+      <c r="B4" s="41" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -70226,8 +70229,8 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="34" t="s">
         <v>178</v>
       </c>
@@ -70257,8 +70260,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40" t="s">
+      <c r="A6" s="41"/>
+      <c r="B6" s="41" t="s">
         <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -70276,8 +70279,8 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="34" t="s">
         <v>178</v>
       </c>
@@ -70295,7 +70298,7 @@
       <c r="M7" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="40" t="s">
+      <c r="A9" s="41" t="s">
         <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -70316,7 +70319,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="40"/>
+      <c r="A10" s="41"/>
       <c r="B10" s="2" t="s">
         <v>160</v>
       </c>
@@ -70337,8 +70340,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="28" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -70354,8 +70357,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
       <c r="C12" s="34" t="s">
         <v>178</v>
       </c>
@@ -70373,7 +70376,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="41" t="s">
         <v>164</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -70408,8 +70411,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="41" t="s">
         <v>165</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -70427,8 +70430,8 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="41"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="34" t="s">
         <v>178</v>
       </c>
@@ -70453,42 +70456,78 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="18" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="39" t="s">
+    <row r="18" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="40" t="s">
         <v>168</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>158</v>
       </c>
+      <c r="C18" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>117</v>
+      </c>
     </row>
-    <row r="19" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="1" t="s">
+    <row r="19" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="40"/>
+      <c r="B19" s="40" t="s">
         <v>169</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
-    <row r="20" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="1" t="s">
+    <row r="20" spans="1:6" s="39" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="40"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D20" s="34" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="39" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="40"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="52"/>
+    </row>
+    <row r="22" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="40"/>
+      <c r="B22" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="1" t="s">
+    <row r="26" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
         <v>167</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A18:A20"/>
+  <mergeCells count="10">
+    <mergeCell ref="A18:A22"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B2:B3"/>
@@ -70497,6 +70536,7 @@
     <mergeCell ref="A1:A7"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Drop Enrollment - Done!
</commit_message>
<xml_diff>
--- a/Tables.xlsx
+++ b/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Edumantra\Binghamton\1. Spring 2018\Database Systems\x2. Project 2\Solution\shree\MiniPods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC417E1-77DB-474E-890F-FCA7A0DD7C0C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7243C709-CFB8-4C57-8FAF-7393DB2C342C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" firstSheet="1" activeTab="8" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9216" tabRatio="834" firstSheet="1" activeTab="6" xr2:uid="{23FB6CCA-2C19-4E54-854E-9BC9CD47D5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="316">
   <si>
     <t>SID</t>
   </si>
@@ -971,6 +971,24 @@
   <si>
     <t>L_Message_EnrollStudent</t>
   </si>
+  <si>
+    <t>T_sid_DropEnrollment</t>
+  </si>
+  <si>
+    <t>T_cid_DropEnrollment</t>
+  </si>
+  <si>
+    <t>B_Drop_DropEnrollment</t>
+  </si>
+  <si>
+    <t>B_Cancel_DropEnrollment</t>
+  </si>
+  <si>
+    <t>L_Error_DropEnrollment</t>
+  </si>
+  <si>
+    <t>L_Message_DropEnrollment</t>
+  </si>
 </sst>
 </file>
 
@@ -1352,13 +1370,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1395,9 +1416,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1989,18 +2007,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
@@ -2027,7 +2045,7 @@
       <c r="J3" s="19"/>
     </row>
     <row r="5" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="44" t="s">
         <v>186</v>
       </c>
       <c r="B5" s="27" t="s">
@@ -2043,12 +2061,12 @@
       <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="44"/>
+      <c r="A6" s="45"/>
       <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="44"/>
-      <c r="B7" s="42" t="s">
+      <c r="A7" s="45"/>
+      <c r="B7" s="43" t="s">
         <v>184</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -2063,8 +2081,8 @@
       <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="44"/>
-      <c r="B8" s="42"/>
+      <c r="A8" s="45"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="20" t="s">
         <v>210</v>
       </c>
@@ -2079,7 +2097,7 @@
       <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="44"/>
+      <c r="A9" s="45"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
@@ -2091,8 +2109,8 @@
       <c r="J9" s="24"/>
     </row>
     <row r="10" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="44"/>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="45"/>
+      <c r="B10" s="43" t="s">
         <v>185</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -2113,8 +2131,8 @@
       <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="44"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="45"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="20" t="s">
         <v>190</v>
       </c>
@@ -2137,8 +2155,8 @@
       <c r="J11" s="19"/>
     </row>
     <row r="12" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="44"/>
-      <c r="B12" s="42"/>
+      <c r="A12" s="45"/>
+      <c r="B12" s="43"/>
       <c r="C12" s="19" t="s">
         <v>204</v>
       </c>
@@ -2153,8 +2171,8 @@
       <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="44"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="43"/>
       <c r="C13" s="19" t="s">
         <v>203</v>
       </c>
@@ -2169,7 +2187,7 @@
       <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="44"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -2181,8 +2199,8 @@
       <c r="J14" s="24"/>
     </row>
     <row r="15" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="44"/>
-      <c r="B15" s="46" t="s">
+      <c r="A15" s="45"/>
+      <c r="B15" s="47" t="s">
         <v>206</v>
       </c>
       <c r="C15" s="19" t="s">
@@ -2197,8 +2215,8 @@
       <c r="J15" s="19"/>
     </row>
     <row r="16" spans="1:10" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="44"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="45"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="19" t="s">
         <v>213</v>
       </c>
@@ -2213,8 +2231,8 @@
       <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="45"/>
+      <c r="B17" s="48"/>
       <c r="C17" s="19" t="s">
         <v>220</v>
       </c>
@@ -2227,8 +2245,8 @@
       <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="44"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="25" t="s">
         <v>216</v>
       </c>
@@ -18629,8 +18647,8 @@
       <c r="XFD18" s="26"/>
     </row>
     <row r="19" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="44"/>
-      <c r="B19" s="47"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="25" t="s">
         <v>217</v>
       </c>
@@ -35021,7 +35039,7 @@
       <c r="XFD19" s="26"/>
     </row>
     <row r="20" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="44"/>
+      <c r="A20" s="45"/>
       <c r="B20" s="22"/>
       <c r="C20" s="23"/>
       <c r="D20" s="23"/>
@@ -35033,8 +35051,8 @@
       <c r="J20" s="24"/>
     </row>
     <row r="21" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="44"/>
-      <c r="B21" s="46" t="s">
+      <c r="A21" s="45"/>
+      <c r="B21" s="47" t="s">
         <v>207</v>
       </c>
       <c r="C21" s="19" t="s">
@@ -35049,8 +35067,8 @@
       <c r="J21" s="19"/>
     </row>
     <row r="22" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="44"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="45"/>
+      <c r="B22" s="48"/>
       <c r="C22" s="19" t="s">
         <v>231</v>
       </c>
@@ -35065,8 +35083,8 @@
       <c r="J22" s="19"/>
     </row>
     <row r="23" spans="1:16384" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="45"/>
-      <c r="B23" s="48"/>
+      <c r="A23" s="46"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="19" t="s">
         <v>229</v>
       </c>
@@ -35110,13 +35128,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
     <row r="2" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -35150,7 +35168,7 @@
       <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="50" t="s">
         <v>241</v>
       </c>
       <c r="B5" s="30" t="s">
@@ -35161,15 +35179,15 @@
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
       <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="42" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="43" t="s">
         <v>243</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -35179,8 +35197,8 @@
       <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="42"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="30" t="s">
         <v>245</v>
       </c>
@@ -35190,15 +35208,15 @@
       <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
       <c r="E9" s="24"/>
     </row>
     <row r="10" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="43" t="s">
         <v>248</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -35208,8 +35226,8 @@
       <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="30" t="s">
         <v>250</v>
       </c>
@@ -35219,15 +35237,15 @@
       <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
+      <c r="A12" s="51"/>
       <c r="B12" s="22"/>
       <c r="C12" s="23"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="46" t="s">
+      <c r="A13" s="51"/>
+      <c r="B13" s="47" t="s">
         <v>247</v>
       </c>
       <c r="C13" s="19" t="s">
@@ -35239,8 +35257,8 @@
       <c r="E13" s="19"/>
     </row>
     <row r="14" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
-      <c r="B14" s="47"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="19" t="s">
         <v>254</v>
       </c>
@@ -35248,8 +35266,8 @@
       <c r="E14" s="19"/>
     </row>
     <row r="15" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="47"/>
+      <c r="A15" s="51"/>
+      <c r="B15" s="48"/>
       <c r="C15" s="19" t="s">
         <v>255</v>
       </c>
@@ -35259,8 +35277,8 @@
       <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="48"/>
       <c r="C16" s="19" t="s">
         <v>257</v>
       </c>
@@ -51642,8 +51660,8 @@
       <c r="XEY16" s="26"/>
     </row>
     <row r="17" spans="1:16379" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="51"/>
-      <c r="B17" s="48"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="30" t="s">
         <v>259</v>
       </c>
@@ -68055,20 +68073,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="43" t="s">
         <v>263</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
     </row>
     <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
@@ -68121,7 +68139,7 @@
       <c r="L4" s="32"/>
     </row>
     <row r="5" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+      <c r="A5" s="50" t="s">
         <v>268</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -68139,7 +68157,7 @@
       <c r="L5" s="19"/>
     </row>
     <row r="6" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
+      <c r="A6" s="51"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
@@ -68153,8 +68171,8 @@
       <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="42" t="s">
+      <c r="A7" s="51"/>
+      <c r="B7" s="43" t="s">
         <v>261</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -68171,8 +68189,8 @@
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="42"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="31" t="s">
         <v>270</v>
       </c>
@@ -68189,22 +68207,22 @@
       <c r="L8" s="19"/>
     </row>
     <row r="9" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
+      <c r="A9" s="51"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
       <c r="J9" s="23"/>
       <c r="K9" s="23"/>
       <c r="L9" s="24"/>
     </row>
     <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="46" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="47" t="s">
         <v>262</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -68221,8 +68239,8 @@
       <c r="L10" s="19"/>
     </row>
     <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="47"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="19" t="s">
         <v>274</v>
       </c>
@@ -68239,8 +68257,8 @@
       <c r="L11" s="19"/>
     </row>
     <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="47"/>
+      <c r="A12" s="51"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="19" t="s">
         <v>276</v>
       </c>
@@ -68255,8 +68273,8 @@
       <c r="L12" s="19"/>
     </row>
     <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="47"/>
+      <c r="A13" s="51"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="33" t="s">
         <v>277</v>
       </c>
@@ -68289,8 +68307,8 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="51"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="33" t="s">
         <v>278</v>
       </c>
@@ -68322,51 +68340,37 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4947D9BD-9EC3-4FDB-A350-33C06B093680}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.77734375" defaultRowHeight="25.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="25.77734375" style="18"/>
-    <col min="3" max="12" width="30.77734375" style="18" customWidth="1"/>
-    <col min="13" max="16384" width="25.77734375" style="18"/>
+    <col min="3" max="5" width="30.77734375" style="18" customWidth="1"/>
+    <col min="6" max="16384" width="25.77734375" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
         <v>290</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
-      <c r="K1" s="42"/>
-      <c r="L1" s="42"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
     </row>
-    <row r="2" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26"/>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
-    <row r="3" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="37" t="s">
+    <row r="3" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="39" t="s">
         <v>291</v>
       </c>
       <c r="B3" s="19" t="s">
@@ -68381,63 +68385,35 @@
       <c r="E3" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
     </row>
-    <row r="4" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="26"/>
       <c r="B4" s="26"/>
       <c r="C4" s="26"/>
       <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="26"/>
-      <c r="K4" s="26"/>
-      <c r="L4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
-    <row r="5" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="49" t="s">
+    <row r="5" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
         <v>296</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="39" t="s">
         <v>297</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
     </row>
-    <row r="6" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
+    <row r="6" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
       <c r="B6" s="22"/>
       <c r="C6" s="26"/>
       <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
-    <row r="7" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="50"/>
-      <c r="B7" s="42" t="s">
+    <row r="7" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="43" t="s">
         <v>298</v>
       </c>
       <c r="C7" s="19" t="s">
@@ -68445,49 +68421,28 @@
       </c>
       <c r="D7" s="19"/>
       <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
     </row>
-    <row r="8" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="50"/>
-      <c r="B8" s="42"/>
-      <c r="C8" s="37" t="s">
+    <row r="8" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="39" t="s">
         <v>300</v>
       </c>
       <c r="D8" s="19" t="s">
         <v>301</v>
       </c>
       <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
     </row>
-    <row r="9" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="50"/>
+    <row r="9" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
       <c r="B9" s="22"/>
       <c r="C9" s="23"/>
       <c r="D9" s="23"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="24"/>
+      <c r="E9" s="24"/>
     </row>
-    <row r="10" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50"/>
-      <c r="B10" s="46" t="s">
+    <row r="10" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="51"/>
+      <c r="B10" s="47" t="s">
         <v>302</v>
       </c>
       <c r="C10" s="19" t="s">
@@ -68497,17 +68452,10 @@
         <v>305</v>
       </c>
       <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
     </row>
-    <row r="11" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="50"/>
-      <c r="B11" s="47"/>
+    <row r="11" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="48"/>
       <c r="C11" s="19" t="s">
         <v>306</v>
       </c>
@@ -68515,151 +68463,81 @@
         <v>307</v>
       </c>
       <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
     </row>
-    <row r="12" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="50"/>
-      <c r="B12" s="47"/>
+    <row r="12" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="19" t="s">
         <v>308</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
     </row>
-    <row r="13" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="50"/>
-      <c r="B13" s="47"/>
+    <row r="13" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="19" t="s">
         <v>309</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="K13" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>287</v>
-      </c>
     </row>
-    <row r="14" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="50"/>
+    <row r="14" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
       <c r="B14" s="22"/>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="24"/>
+      <c r="E14" s="24"/>
     </row>
-    <row r="15" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="50"/>
-      <c r="B15" s="46" t="s">
+    <row r="15" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="51"/>
+      <c r="B15" s="47" t="s">
         <v>303</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
+      <c r="C15" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>311</v>
+      </c>
       <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
     </row>
-    <row r="16" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="50"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="19"/>
+    <row r="16" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>313</v>
+      </c>
       <c r="E16" s="19"/>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
     </row>
-    <row r="17" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="50"/>
-      <c r="B17" s="47"/>
-      <c r="C17" s="19"/>
+    <row r="17" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="48"/>
+      <c r="C17" s="19" t="s">
+        <v>314</v>
+      </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
     </row>
-    <row r="18" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="50"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="37"/>
+    <row r="18" spans="1:5" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="52"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="19" t="s">
+        <v>315</v>
+      </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="K18" s="19" t="s">
-        <v>286</v>
-      </c>
-      <c r="L18" s="19" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:E1"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="A5:A19"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A5:A18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -69820,9 +69698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718F9279-C340-4770-88F1-01842C5185FC}">
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="22.05" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -70112,7 +69990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4014D9C3-5F07-4F82-A3CA-A19916A85FB5}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -70129,7 +70007,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="42" t="s">
         <v>157</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -70164,8 +70042,8 @@
       <c r="M1" s="9"/>
     </row>
     <row r="2" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41" t="s">
+      <c r="A2" s="42"/>
+      <c r="B2" s="42" t="s">
         <v>161</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -70193,8 +70071,8 @@
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41"/>
-      <c r="B3" s="41"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
       <c r="C3" s="34" t="s">
         <v>178</v>
       </c>
@@ -70210,8 +70088,8 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="41"/>
-      <c r="B4" s="41" t="s">
+      <c r="A4" s="42"/>
+      <c r="B4" s="42" t="s">
         <v>162</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -70229,8 +70107,8 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41"/>
-      <c r="B5" s="41"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="42"/>
       <c r="C5" s="34" t="s">
         <v>178</v>
       </c>
@@ -70260,8 +70138,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41" t="s">
+      <c r="A6" s="42"/>
+      <c r="B6" s="42" t="s">
         <v>171</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -70279,8 +70157,8 @@
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="42"/>
       <c r="C7" s="34" t="s">
         <v>178</v>
       </c>
@@ -70298,7 +70176,7 @@
       <c r="M7" s="7"/>
     </row>
     <row r="9" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="42" t="s">
         <v>159</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -70319,7 +70197,7 @@
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="41"/>
+      <c r="A10" s="42"/>
       <c r="B10" s="2" t="s">
         <v>160</v>
       </c>
@@ -70340,8 +70218,8 @@
       </c>
     </row>
     <row r="11" spans="1:13" s="28" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="42" t="s">
         <v>163</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -70357,8 +70235,8 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="42"/>
       <c r="C12" s="34" t="s">
         <v>178</v>
       </c>
@@ -70376,7 +70254,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="42" t="s">
         <v>164</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -70411,8 +70289,8 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="41"/>
-      <c r="B15" s="41" t="s">
+      <c r="A15" s="42"/>
+      <c r="B15" s="42" t="s">
         <v>165</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -70430,8 +70308,8 @@
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:13" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="41"/>
-      <c r="B16" s="41"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="34" t="s">
         <v>178</v>
       </c>
@@ -70457,7 +70335,7 @@
       <c r="K16" s="2"/>
     </row>
     <row r="18" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="41" t="s">
         <v>168</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -70477,8 +70355,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40" t="s">
+      <c r="A19" s="41"/>
+      <c r="B19" s="41" t="s">
         <v>169</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -70491,9 +70369,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="39" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40"/>
-      <c r="B20" s="40"/>
+    <row r="20" spans="1:6" s="38" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="41"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="7" t="s">
         <v>178</v>
       </c>
@@ -70501,13 +70379,13 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:6" s="39" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="40"/>
+    <row r="21" spans="1:6" s="38" customFormat="1" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="41"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="52"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="40"/>
+      <c r="A22" s="41"/>
       <c r="B22" s="1" t="s">
         <v>170</v>
       </c>

</xml_diff>